<commit_message>
Update 3-7 repeated purchase exercise.xlsx
</commit_message>
<xml_diff>
--- a/Marketing Analytics in Python/Bass model/Dataset/3-7 repeated purchase exercise.xlsx
+++ b/Marketing Analytics in Python/Bass model/Dataset/3-7 repeated purchase exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zoutianxin\Documents\GitHub\MarketingAnalyticsPython\Marketing Analytics in Python\Bass model\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28114C63-C641-499A-96D8-C346D19A3A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C472AD-6874-413E-B8A9-BDCCCCA38268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -362,7 +362,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -380,7 +380,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>19.877359388566205</v>
+        <v>19.966807505814753</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -388,7 +388,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>69.225544027751582</v>
+        <v>71.717663612750641</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -396,7 +396,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>142.19567902127659</v>
+        <v>145.82166883631916</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -404,7 +404,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>249.47826047834269</v>
+        <v>242.36813005470995</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -412,7 +412,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>405.88813807283555</v>
+        <v>390.66733289510421</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -420,7 +420,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>631.15802033964485</v>
+        <v>622.63738706505967</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -428,7 +428,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>949.99067484762691</v>
+        <v>953.79063754701747</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -436,7 +436,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1390.3296235876187</v>
+        <v>1338.1922627030831</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -444,7 +444,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>1978.4760656941282</v>
+        <v>1991.33616012114</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -452,7 +452,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>2730.1709590331093</v>
+        <v>2863.9493360257316</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -460,7 +460,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>3639.0215491851532</v>
+        <v>3518.9338380620434</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -468,7 +468,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>4667.5317016755052</v>
+        <v>4653.5291065704787</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -476,7 +476,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>5748.3535790990463</v>
+        <v>5952.4201311570623</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -484,7 +484,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>6799.4701784445697</v>
+        <v>6850.4662047829042</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -492,7 +492,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>7747.3134704595177</v>
+        <v>7774.4290676061264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>